<commit_message>
update impfdaten manually for corona report
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-01-24.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-01-24.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="322">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -739,10 +739,10 @@
     <t xml:space="preserve">Geimpfte Personen</t>
   </si>
   <si>
-    <t xml:space="preserve">Stand 19.1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stand 26.1.</t>
+    <t xml:space="preserve">Stand 20.1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stand 27.1.</t>
   </si>
   <si>
     <t xml:space="preserve">fdsa</t>
@@ -775,217 +775,226 @@
     <t xml:space="preserve">7-Tage-Inzidenz 80+</t>
   </si>
   <si>
-    <t xml:space="preserve">52,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,0</t>
+    <t xml:space="preserve">51,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,4</t>
   </si>
   <si>
     <t xml:space="preserve">1,4</t>
   </si>
   <si>
-    <t xml:space="preserve">1,6</t>
-  </si>
-  <si>
     <t xml:space="preserve">0,3</t>
   </si>
   <si>
-    <t xml:space="preserve">31,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,8</t>
+    <t xml:space="preserve">41,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,0</t>
   </si>
   <si>
     <t xml:space="preserve">1,9</t>
   </si>
   <si>
-    <t xml:space="preserve">40,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,1</t>
+    <t xml:space="preserve">1,2</t>
   </si>
   <si>
     <t xml:space="preserve">0,5</t>
   </si>
   <si>
-    <t xml:space="preserve">49,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,9</t>
+    <t xml:space="preserve">82,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,1</t>
   </si>
   <si>
     <t xml:space="preserve">1,7</t>
   </si>
   <si>
-    <t xml:space="preserve">0,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6,0</t>
+    <t xml:space="preserve">37,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,9</t>
   </si>
   <si>
     <t xml:space="preserve">2,8</t>
   </si>
   <si>
-    <t xml:space="preserve">0,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,8</t>
+    <t xml:space="preserve">22,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,0</t>
   </si>
 </sst>
 </file>
@@ -1464,13 +1473,13 @@
         <v>251</v>
       </c>
       <c r="F2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2" t="s">
         <v>252</v>
       </c>
-      <c r="G2" t="s">
-        <v>253</v>
-      </c>
       <c r="H2" t="n">
-        <v>1921689</v>
+        <v>1990889</v>
       </c>
       <c r="I2" t="n">
         <v>103</v>
@@ -1484,25 +1493,25 @@
         <v>154</v>
       </c>
       <c r="B3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" t="s">
         <v>254</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" t="s">
         <v>255</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>256</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>257</v>
       </c>
-      <c r="F3" t="s">
-        <v>251</v>
-      </c>
-      <c r="G3" t="s">
-        <v>253</v>
-      </c>
       <c r="H3" t="n">
-        <v>210862</v>
+        <v>228138</v>
       </c>
       <c r="I3" t="n">
         <v>82</v>
@@ -1534,7 +1543,7 @@
         <v>263</v>
       </c>
       <c r="H4" t="n">
-        <v>384311</v>
+        <v>365003</v>
       </c>
       <c r="I4" t="n">
         <v>98</v>
@@ -1560,13 +1569,13 @@
         <v>267</v>
       </c>
       <c r="F5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G5" t="s">
         <v>268</v>
       </c>
       <c r="H5" t="n">
-        <v>97855</v>
+        <v>103639</v>
       </c>
       <c r="I5" t="n">
         <v>94</v>
@@ -1595,10 +1604,10 @@
         <v>273</v>
       </c>
       <c r="G6" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="H6" t="n">
-        <v>63024</v>
+        <v>68478</v>
       </c>
       <c r="I6" t="n">
         <v>150</v>
@@ -1612,25 +1621,25 @@
         <v>163</v>
       </c>
       <c r="B7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D7" t="s">
-        <v>232</v>
+        <v>277</v>
       </c>
       <c r="E7" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="F7" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H7" t="n">
-        <v>18597</v>
+        <v>19825</v>
       </c>
       <c r="I7" t="n">
         <v>78</v>
@@ -1644,25 +1653,25 @@
         <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C8" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D8" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E8" t="s">
         <v>251</v>
       </c>
       <c r="F8" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="G8" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
       <c r="H8" t="n">
-        <v>40597</v>
+        <v>44231</v>
       </c>
       <c r="I8" t="n">
         <v>88</v>
@@ -1676,25 +1685,25 @@
         <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E9" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="F9" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="G9" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="H9" t="n">
-        <v>133933</v>
+        <v>141478</v>
       </c>
       <c r="I9" t="n">
         <v>105</v>
@@ -1708,25 +1717,25 @@
         <v>171</v>
       </c>
       <c r="B10" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C10" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D10" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E10" t="s">
         <v>268</v>
       </c>
       <c r="F10" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="G10" t="s">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="H10" t="n">
-        <v>57008</v>
+        <v>62212</v>
       </c>
       <c r="I10" t="n">
         <v>103</v>
@@ -1740,25 +1749,25 @@
         <v>174</v>
       </c>
       <c r="B11" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C11" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D11" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E11" t="s">
         <v>268</v>
       </c>
       <c r="F11" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="G11" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H11" t="n">
-        <v>143881</v>
+        <v>152734</v>
       </c>
       <c r="I11" t="n">
         <v>79</v>
@@ -1772,25 +1781,25 @@
         <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C12" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D12" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E12" t="s">
         <v>272</v>
       </c>
       <c r="F12" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="G12" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="H12" t="n">
-        <v>346136</v>
+        <v>357370</v>
       </c>
       <c r="I12" t="n">
         <v>98</v>
@@ -1804,25 +1813,25 @@
         <v>178</v>
       </c>
       <c r="B13" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C13" t="s">
-        <v>300</v>
+        <v>234</v>
       </c>
       <c r="D13" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E13" t="s">
         <v>272</v>
       </c>
       <c r="F13" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G13" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="H13" t="n">
-        <v>134151</v>
+        <v>139626</v>
       </c>
       <c r="I13" t="n">
         <v>98</v>
@@ -1836,25 +1845,25 @@
         <v>180</v>
       </c>
       <c r="B14" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C14" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D14" t="s">
-        <v>278</v>
+        <v>306</v>
       </c>
       <c r="E14" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="F14" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="G14" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="H14" t="n">
-        <v>22738</v>
+        <v>24255</v>
       </c>
       <c r="I14" t="n">
         <v>108</v>
@@ -1868,25 +1877,25 @@
         <v>183</v>
       </c>
       <c r="B15" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C15" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D15" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E15" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="F15" t="s">
-        <v>280</v>
+        <v>311</v>
       </c>
       <c r="G15" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="H15" t="n">
-        <v>80086</v>
+        <v>86187</v>
       </c>
       <c r="I15" t="n">
         <v>144</v>
@@ -1900,25 +1909,25 @@
         <v>186</v>
       </c>
       <c r="B16" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C16" t="s">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="D16" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E16" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="F16" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="G16" t="s">
-        <v>313</v>
+        <v>263</v>
       </c>
       <c r="H16" t="n">
-        <v>56802</v>
+        <v>59750</v>
       </c>
       <c r="I16" t="n">
         <v>194</v>
@@ -1938,19 +1947,19 @@
         <v>315</v>
       </c>
       <c r="D17" t="s">
-        <v>278</v>
+        <v>306</v>
       </c>
       <c r="E17" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
       <c r="F17" t="s">
-        <v>289</v>
+        <v>317</v>
       </c>
       <c r="G17" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="H17" t="n">
-        <v>88331</v>
+        <v>91473</v>
       </c>
       <c r="I17" t="n">
         <v>93</v>
@@ -1964,25 +1973,25 @@
         <v>191</v>
       </c>
       <c r="B18" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C18" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D18" t="s">
-        <v>260</v>
+        <v>320</v>
       </c>
       <c r="E18" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="F18" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="G18" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="H18" t="n">
-        <v>43377</v>
+        <v>46490</v>
       </c>
       <c r="I18" t="n">
         <v>186</v>

</xml_diff>